<commit_message>
Adding more things for sensitivity and the final report outline
</commit_message>
<xml_diff>
--- a/LCA/mass_balances_lca.xlsx
+++ b/LCA/mass_balances_lca.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Χαρακτηρισμός της τροφοδοσίας" sheetId="1" state="visible" r:id="rId3"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="124">
   <si>
     <t xml:space="preserve">Ισοζύγια μάζας</t>
   </si>
@@ -254,6 +254,9 @@
   </si>
   <si>
     <t xml:space="preserve">Ποσοστό λιγνίνης στην κυτταρινική φάση</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ανάκτηση ημικυτταρίνης</t>
   </si>
   <si>
     <t xml:space="preserve">Γλυκόζη από υδρόλυση (% dry substrate)</t>
@@ -621,7 +624,7 @@
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B35" activeCellId="1" sqref="B11:D12 B35"/>
+      <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1045,10 +1048,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="1" sqref="B11:D12 C15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A47" activeCellId="0" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1462,7 +1465,8 @@
         <v>77</v>
       </c>
       <c r="B46" s="1" t="n">
-        <v>0.309</v>
+        <f aca="false">C22/B6</f>
+        <v>0.494603773584905</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1470,49 +1474,45 @@
         <v>78</v>
       </c>
       <c r="B47" s="1" t="n">
-        <f aca="false">C15*B46</f>
-        <v>1.91076344881648</v>
+        <v>0.309</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B48" s="3" t="n">
-        <f aca="false">0.02/100*B40</f>
-        <v>0.000707042208972231</v>
+      <c r="B48" s="1" t="n">
+        <f aca="false">C15*B47</f>
+        <v>1.91076344881648</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B49" s="1" t="n">
-        <f aca="false">B10-B48</f>
+      <c r="B49" s="3" t="n">
+        <f aca="false">0.02/100*B40</f>
+        <v>0.000707042208972231</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B50" s="1" t="n">
+        <f aca="false">B10-B49</f>
         <v>0.0460506173872979</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B52" s="1" t="n">
-        <v>0.457</v>
-      </c>
-      <c r="C52" s="1" t="n">
-        <f aca="false">B52*$C$14</f>
-        <v>1.36222596526283</v>
+      <c r="C52" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1520,35 +1520,35 @@
         <v>84</v>
       </c>
       <c r="B53" s="1" t="n">
-        <v>0.0222</v>
+        <v>0.457</v>
       </c>
       <c r="C53" s="1" t="n">
         <f aca="false">B53*$C$14</f>
-        <v>0.0661737777436213</v>
+        <v>1.36222596526283</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B54" s="2" t="n">
-        <v>0.009</v>
+      <c r="B54" s="1" t="n">
+        <v>0.0222</v>
       </c>
       <c r="C54" s="1" t="n">
         <f aca="false">B54*$C$14</f>
-        <v>0.02682720719336</v>
+        <v>0.0661737777436213</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B55" s="1" t="n">
-        <v>0.0118</v>
+      <c r="B55" s="2" t="n">
+        <v>0.009</v>
       </c>
       <c r="C55" s="1" t="n">
         <f aca="false">B55*$C$14</f>
-        <v>0.0351734494312942</v>
+        <v>0.02682720719336</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1556,32 +1556,44 @@
         <v>87</v>
       </c>
       <c r="B56" s="1" t="n">
-        <v>0.0136</v>
+        <v>0.0118</v>
       </c>
       <c r="C56" s="1" t="n">
         <f aca="false">B56*$C$14</f>
+        <v>0.0351734494312942</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B57" s="1" t="n">
+        <v>0.0136</v>
+      </c>
+      <c r="C57" s="1" t="n">
+        <f aca="false">B57*$C$14</f>
         <v>0.0405388908699662</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C57" s="1" t="n">
-        <f aca="false">SUM(C53:C56)</f>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C58" s="1" t="n">
+        <f aca="false">SUM(C54:C57)</f>
         <v>0.168713325238242</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="n">
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="n">
         <f aca="false">60485.7+45314.4+2182.8+23307+2886.6+1285.2+20547.9+43990.4</f>
         <v>200000</v>
       </c>
-      <c r="B58" s="1" t="n">
-        <f aca="false">B4-A58</f>
+      <c r="B59" s="1" t="n">
+        <f aca="false">B4-A59</f>
         <v>-199988.310585101</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="1" t="n">
-        <f aca="false">C34+B58</f>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="1" t="n">
+        <f aca="false">C34+B59</f>
         <v>-199985.785671483</v>
       </c>
     </row>
@@ -1604,7 +1616,7 @@
   <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P37" activeCellId="1" sqref="B11:D12 P37"/>
+      <selection pane="topLeft" activeCell="P37" activeCellId="0" sqref="P37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1616,7 +1628,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1626,7 +1638,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>60485.68</v>
@@ -1634,7 +1646,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>32692.2</v>
@@ -1642,12 +1654,12 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>230.44</v>
@@ -1655,7 +1667,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>2</v>
@@ -1663,7 +1675,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>4</v>
@@ -1671,12 +1683,12 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>60</v>
@@ -1684,7 +1696,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>28</v>
@@ -1692,7 +1704,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B14" s="1" t="n">
         <f aca="false">B13/B12</f>
@@ -1701,7 +1713,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>0.5</v>
@@ -1709,7 +1721,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B16" s="1" t="n">
         <f aca="false">B15*B14</f>
@@ -1718,12 +1730,12 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B19" s="1" t="n">
         <v>0.0394</v>
@@ -1731,7 +1743,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B20" s="1" t="n">
         <v>2</v>
@@ -1739,7 +1751,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B21" s="1" t="n">
         <f aca="false">B20*B19</f>
@@ -1748,7 +1760,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B23" s="1" t="n">
         <f aca="false">0.004*B4</f>
@@ -1757,7 +1769,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B25" s="1" t="n">
         <f aca="false">B21+B16</f>
@@ -1766,7 +1778,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B26" s="1" t="n">
         <v>1301.5</v>
@@ -1774,7 +1786,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B27" s="1" t="n">
         <v>109</v>
@@ -1782,7 +1794,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B28" s="1" t="n">
         <f aca="false">B25*B26*B27/1000 + B23</f>
@@ -1791,12 +1803,12 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B31" s="1" t="n">
         <v>30400</v>
@@ -1804,7 +1816,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B32" s="1" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(B31-B28)</f>
@@ -1813,7 +1825,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B33" s="1" t="n">
         <v>23.5</v>
@@ -1821,7 +1833,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B34" s="1" t="n">
         <f aca="false">B32*B33/1000</f>
@@ -1846,8 +1858,8 @@
   </sheetPr>
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="B11:D12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1859,7 +1871,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B1" s="1" t="n">
         <f aca="false">11.6894148990675+11.6894148990675/2</f>
@@ -1868,7 +1880,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>3.53521104486115</v>
@@ -1880,7 +1892,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>2.64848943674557</v>
@@ -1892,7 +1904,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>1.36222596526283</v>
@@ -1904,7 +1916,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>0.169905645557946</v>
@@ -1916,7 +1928,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>0.075116180141408</v>
@@ -1928,7 +1940,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B7" s="1" t="n">
         <f aca="false">1.09191826987218+11.6894148990675/2</f>
@@ -1941,7 +1953,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>2.75979069703014</v>
@@ -1953,7 +1965,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>0.0467576595962701</v>

</xml_diff>